<commit_message>
romain - mise a jour fichier roles
</commit_message>
<xml_diff>
--- a/Etat_des_lieux.xlsx
+++ b/Etat_des_lieux.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sesa466660\Documents\Projet_frelons\Projet-frelons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{165CB566-B5F7-4F0E-BF5B-8FB80B74A182}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4313EFCE-BC27-4DC1-9698-A7ACBF899C73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{301318C4-AB70-49FE-8CF5-5892BD3503CB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>ETAT DES LIEUX</t>
   </si>
@@ -48,6 +48,60 @@
   </si>
   <si>
     <t>Commentaires</t>
+  </si>
+  <si>
+    <t>Caméra + vision / traitement image</t>
+  </si>
+  <si>
+    <t>Laser</t>
+  </si>
+  <si>
+    <t>Servo moteur</t>
+  </si>
+  <si>
+    <t>Calcul coordonnées</t>
+  </si>
+  <si>
+    <t>Voir comment on prend des photos, le format de retour, comment on traite les images …</t>
+  </si>
+  <si>
+    <t>Conso du laser, essai de tir</t>
+  </si>
+  <si>
+    <t>Améliorations</t>
+  </si>
+  <si>
+    <t>Raspberry Pi3 ? Se renseigner, Consommation système</t>
+  </si>
+  <si>
+    <t>Arnaud</t>
+  </si>
+  <si>
+    <t>Gilbert</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Alimentation gestion de l'énergie</t>
+  </si>
+  <si>
+    <t>Tous par la suite</t>
+  </si>
+  <si>
+    <t>Comprendre méthode de calcul et essai basique en statique</t>
+  </si>
+  <si>
+    <t>Romain/Antoine</t>
+  </si>
+  <si>
+    <t>Kevin / Gilbert</t>
+  </si>
+  <si>
+    <t>Voir comment fonctionne les moteurs + controller, temps de calibrage, reaction des moteurs</t>
+  </si>
+  <si>
+    <t>Faire le bilan des puissances et regarder si ce qui a été fait est cohérent ou non - calcul autonomie (alimentation a découpage - regulateur)</t>
   </si>
 </sst>
 </file>
@@ -77,7 +131,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -100,23 +154,181 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -435,10 +647,13 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B7"/>
+      <selection activeCell="G17" sqref="G17:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="16384" width="10.90625" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -476,346 +691,370 @@
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4" t="s">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="15"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="19"/>
+      <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="12"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="17"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="A11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="8"/>
+      <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="15"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="A14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="8"/>
+      <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="15"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="A17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="23"/>
+      <c r="I17" s="24"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="27"/>
+    </row>
+    <row r="19" spans="1:9" ht="53.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="14"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="30"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
+      <c r="A20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="8"/>
+      <c r="I20" s="5"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="15"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="7"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="12"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="17"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="7"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="12"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="17"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="7"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="12"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
+      <c r="A31" s="16"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="17"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
+      <c r="A32" s="20"/>
+      <c r="B32" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="G23:I25"/>
-    <mergeCell ref="G26:I28"/>
-    <mergeCell ref="G29:I31"/>
-    <mergeCell ref="C26:D28"/>
-    <mergeCell ref="E26:F28"/>
-    <mergeCell ref="C29:D31"/>
-    <mergeCell ref="E29:F31"/>
-    <mergeCell ref="G5:I7"/>
-    <mergeCell ref="G8:I10"/>
-    <mergeCell ref="G11:I13"/>
-    <mergeCell ref="G14:I16"/>
-    <mergeCell ref="G17:I19"/>
-    <mergeCell ref="G20:I22"/>
-    <mergeCell ref="C17:D19"/>
-    <mergeCell ref="E17:F19"/>
-    <mergeCell ref="C20:D22"/>
-    <mergeCell ref="E20:F22"/>
-    <mergeCell ref="C23:D25"/>
-    <mergeCell ref="E23:F25"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="A1:I3"/>
+    <mergeCell ref="A5:B7"/>
+    <mergeCell ref="A8:B10"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
     <mergeCell ref="A29:B31"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="C5:D7"/>
@@ -832,13 +1071,25 @@
     <mergeCell ref="A20:B22"/>
     <mergeCell ref="A23:B25"/>
     <mergeCell ref="A26:B28"/>
-    <mergeCell ref="A5:B7"/>
-    <mergeCell ref="A8:B10"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="A1:I3"/>
+    <mergeCell ref="G20:I22"/>
+    <mergeCell ref="C17:D19"/>
+    <mergeCell ref="E17:F19"/>
+    <mergeCell ref="C20:D22"/>
+    <mergeCell ref="E20:F22"/>
+    <mergeCell ref="G5:I7"/>
+    <mergeCell ref="G8:I10"/>
+    <mergeCell ref="G11:I13"/>
+    <mergeCell ref="G14:I16"/>
+    <mergeCell ref="G17:I19"/>
+    <mergeCell ref="G23:I25"/>
+    <mergeCell ref="G26:I28"/>
+    <mergeCell ref="G29:I31"/>
+    <mergeCell ref="C26:D28"/>
+    <mergeCell ref="E26:F28"/>
+    <mergeCell ref="C29:D31"/>
+    <mergeCell ref="E29:F31"/>
+    <mergeCell ref="C23:D25"/>
+    <mergeCell ref="E23:F25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>